<commit_message>
Week 9 overzicht - Draft
</commit_message>
<xml_diff>
--- a/weekoverzichten/Stage - Week 9.xlsx
+++ b/weekoverzichten/Stage - Week 9.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Maandag</t>
   </si>
@@ -39,6 +39,30 @@
   </si>
   <si>
     <t>Vrijdag</t>
+  </si>
+  <si>
+    <t>Werken aan document</t>
+  </si>
+  <si>
+    <t>Keras implementeren</t>
+  </si>
+  <si>
+    <t>Keras problemen oplossen</t>
+  </si>
+  <si>
+    <t>Meeting, code bespreken</t>
+  </si>
+  <si>
+    <t>Keras verder implementeren</t>
+  </si>
+  <si>
+    <t>Keras op MNIST laten werken</t>
+  </si>
+  <si>
+    <t>Automatisch Learning Rate veranderen</t>
+  </si>
+  <si>
+    <t>Recurrent Neural Networks onderzoeken</t>
   </si>
 </sst>
 </file>
@@ -89,7 +113,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -100,6 +124,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,7 +441,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -445,24 +472,46 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="2"/>
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="A3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
+      <c r="A4" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
+      <c r="C4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>